<commit_message>
Update to DSR release estimates
</commit_message>
<xml_diff>
--- a/output/reports/SE_RF_HowMth_thru2023.xlsx
+++ b/output/reports/SE_RF_HowMth_thru2023.xlsx
@@ -167,8 +167,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-        </a:blip>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">        </a:blip>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -317,6 +316,36 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+    <xdr:from xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+      <xdr:col xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">11</xdr:col>
+      <xdr:colOff xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:colOff>
+      <xdr:row xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:row>
+      <xdr:rowOff xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" cx="9144000" cy="6400800"/>
+    <xdr:pic xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+      <xdr:nvPicPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+        <xdr:cNvPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" id="2" name="Picture 2"/>
+        <xdr:cNvPicPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        </a:blip>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -339,6 +368,36 @@
       </xdr:nvPicPr>
       <xdr:blipFill xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
         <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">        </a:blip>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+    <xdr:from xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+      <xdr:col xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">11</xdr:col>
+      <xdr:colOff xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:colOff>
+      <xdr:row xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:row>
+      <xdr:rowOff xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" cx="9144000" cy="6400800"/>
+    <xdr:pic xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+      <xdr:nvPicPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+        <xdr:cNvPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" id="2" name="Picture 2"/>
+        <xdr:cNvPicPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        </a:blip>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -440,8 +499,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-        </a:blip>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">        </a:blip>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>

</xml_diff>

<commit_message>
Fixed DSR release estimates
</commit_message>
<xml_diff>
--- a/output/reports/SE_RF_HowMth_thru2023.xlsx
+++ b/output/reports/SE_RF_HowMth_thru2023.xlsx
@@ -332,6 +332,35 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">        </a:blip>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+    <xdr:from xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+      <xdr:col xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">11</xdr:col>
+      <xdr:colOff xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:colOff>
+      <xdr:row xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:row>
+      <xdr:rowOff xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" cx="9144000" cy="6400800"/>
+    <xdr:pic xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+      <xdr:nvPicPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+        <xdr:cNvPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" id="2" name="Picture 2"/>
+        <xdr:cNvPicPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
         <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
         </a:blip>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -368,6 +397,35 @@
       </xdr:nvPicPr>
       <xdr:blipFill xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
         <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">        </a:blip>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+    <xdr:from xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+      <xdr:col xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">11</xdr:col>
+      <xdr:colOff xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:colOff>
+      <xdr:row xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:row>
+      <xdr:rowOff xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" cx="9144000" cy="6400800"/>
+    <xdr:pic xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+      <xdr:nvPicPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+        <xdr:cNvPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" id="2" name="Picture 2"/>
+        <xdr:cNvPicPr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">        </a:blip>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -24613,10 +24671,10 @@
         <v>2023</v>
       </c>
       <c r="D53" t="n">
-        <v>121</v>
+        <v>119.574410352807</v>
       </c>
       <c r="E53" t="n">
-        <v>0</v>
+        <v>2.62603259368155</v>
       </c>
       <c r="F53" t="n">
         <v>109.36018196705</v>
@@ -24625,10 +24683,10 @@
         <v>55.7251435848831</v>
       </c>
       <c r="H53" t="n">
-        <v>230.36018196705</v>
+        <v>228.934592319857</v>
       </c>
       <c r="I53" t="n">
-        <v>55.7251435848831</v>
+        <v>55.7869848149092</v>
       </c>
     </row>
     <row r="54">
@@ -28351,22 +28409,22 @@
         <v>2022</v>
       </c>
       <c r="D25" t="n">
-        <v>355.475806451613</v>
+        <v>5534.26916859248</v>
       </c>
       <c r="E25" t="n">
-        <v>14.8380468085321</v>
+        <v>397.232080850614</v>
       </c>
       <c r="F25" t="n">
-        <v>1616.94833090028</v>
+        <v>1634.15804586966</v>
       </c>
       <c r="G25" t="n">
-        <v>1067.13137003996</v>
+        <v>1078.48920155647</v>
       </c>
       <c r="H25" t="n">
-        <v>1972.4241373519</v>
+        <v>7168.42721446213</v>
       </c>
       <c r="I25" t="n">
-        <v>1067.2345236903</v>
+        <v>1149.31818219796</v>
       </c>
     </row>
     <row r="26">
@@ -28380,10 +28438,10 @@
         <v>2023</v>
       </c>
       <c r="D26" t="n">
-        <v>163.049261083744</v>
+        <v>5133.5026542399</v>
       </c>
       <c r="E26" t="n">
-        <v>8.93783321509818</v>
+        <v>368.466346553666</v>
       </c>
       <c r="F26" t="n">
         <v>2681.74733049403</v>
@@ -28392,10 +28450,10 @@
         <v>1485.69458278873</v>
       </c>
       <c r="H26" t="n">
-        <v>2844.79659157777</v>
+        <v>7815.24998473393</v>
       </c>
       <c r="I26" t="n">
-        <v>1485.72146723078</v>
+        <v>1530.70436135473</v>
       </c>
     </row>
     <row r="27">
@@ -29074,10 +29132,10 @@
         <v>2022</v>
       </c>
       <c r="D50" t="n">
-        <v>663.09445741102</v>
+        <v>809.350760983049</v>
       </c>
       <c r="E50" t="n">
-        <v>14.5625443831432</v>
+        <v>17.7745511919437</v>
       </c>
       <c r="F50" t="n">
         <v>63.5772864145279</v>
@@ -29086,10 +29144,10 @@
         <v>237.911947243354</v>
       </c>
       <c r="H50" t="n">
-        <v>726.671743825548</v>
+        <v>872.928047397577</v>
       </c>
       <c r="I50" t="n">
-        <v>238.357215833789</v>
+        <v>238.574997246567</v>
       </c>
     </row>
     <row r="51">
@@ -29797,10 +29855,10 @@
         <v>2022</v>
       </c>
       <c r="D75" t="n">
-        <v>313.178294573643</v>
+        <v>2067.8228575235</v>
       </c>
       <c r="E75" t="n">
-        <v>15.4631026042401</v>
+        <v>306.769849936414</v>
       </c>
       <c r="F75" t="n">
         <v>3948.65879948157</v>
@@ -29809,10 +29867,10 @@
         <v>3890.59499715179</v>
       </c>
       <c r="H75" t="n">
-        <v>4261.83709405522</v>
+        <v>6016.48165700507</v>
       </c>
       <c r="I75" t="n">
-        <v>3890.62572594753</v>
+        <v>3902.67051808022</v>
       </c>
     </row>
     <row r="76">
@@ -29826,10 +29884,10 @@
         <v>2023</v>
       </c>
       <c r="D76" t="n">
-        <v>201.230769230769</v>
+        <v>2142.3463743689</v>
       </c>
       <c r="E76" t="n">
-        <v>16.6969180961183</v>
+        <v>317.825713835113</v>
       </c>
       <c r="F76" t="n">
         <v>2287.5574205307</v>
@@ -29838,10 +29896,10 @@
         <v>1968.93053186201</v>
       </c>
       <c r="H76" t="n">
-        <v>2488.78818976147</v>
+        <v>4429.9037948996</v>
       </c>
       <c r="I76" t="n">
-        <v>1969.00132716368</v>
+        <v>1994.41736446342</v>
       </c>
     </row>
     <row r="77">
@@ -30520,10 +30578,10 @@
         <v>2022</v>
       </c>
       <c r="D100" t="n">
-        <v>0</v>
+        <v>2164.44518928065</v>
       </c>
       <c r="E100" t="n">
-        <v>0</v>
+        <v>138.109809111195</v>
       </c>
       <c r="F100" t="n">
         <v>537.722249935495</v>
@@ -30532,10 +30590,10 @@
         <v>784.00794558497</v>
       </c>
       <c r="H100" t="n">
-        <v>537.722249935495</v>
+        <v>2702.16743921614</v>
       </c>
       <c r="I100" t="n">
-        <v>784.00794558497</v>
+        <v>796.079630510099</v>
       </c>
     </row>
     <row r="101">
@@ -30549,10 +30607,10 @@
         <v>2023</v>
       </c>
       <c r="D101" t="n">
-        <v>103.121387283237</v>
+        <v>1629.95787998171</v>
       </c>
       <c r="E101" t="n">
-        <v>8.08912543604989</v>
+        <v>104.005022986227</v>
       </c>
       <c r="F101" t="n">
         <v>1778.44150843085</v>
@@ -30561,10 +30619,10 @@
         <v>2981.58815225084</v>
       </c>
       <c r="H101" t="n">
-        <v>1881.56289571409</v>
+        <v>3408.39938841256</v>
       </c>
       <c r="I101" t="n">
-        <v>2981.59912523345</v>
+        <v>2983.40157445305</v>
       </c>
     </row>
     <row r="102">
@@ -31243,10 +31301,10 @@
         <v>2022</v>
       </c>
       <c r="D125" t="n">
-        <v>462.911214953271</v>
+        <v>6076.73123798912</v>
       </c>
       <c r="E125" t="n">
-        <v>38.2875956764026</v>
+        <v>228.387831137087</v>
       </c>
       <c r="F125" t="n">
         <v>13556.111626549</v>
@@ -31255,10 +31313,10 @@
         <v>5311.82572385114</v>
       </c>
       <c r="H125" t="n">
-        <v>14019.0228415023</v>
+        <v>19632.8428645381</v>
       </c>
       <c r="I125" t="n">
-        <v>5311.96371039462</v>
+        <v>5316.73335065604</v>
       </c>
     </row>
     <row r="126">
@@ -31272,10 +31330,10 @@
         <v>2023</v>
       </c>
       <c r="D126" t="n">
-        <v>625.08908045977</v>
+        <v>9481.1250945404</v>
       </c>
       <c r="E126" t="n">
-        <v>58.6639503098643</v>
+        <v>356.338549834902</v>
       </c>
       <c r="F126" t="n">
         <v>12639.4350128953</v>
@@ -31284,10 +31342,10 @@
         <v>5402.52170647347</v>
       </c>
       <c r="H126" t="n">
-        <v>13264.524093355</v>
+        <v>22120.5601074357</v>
       </c>
       <c r="I126" t="n">
-        <v>5402.84020196627</v>
+        <v>5414.26060981695</v>
       </c>
     </row>
     <row r="127">
@@ -31966,10 +32024,10 @@
         <v>2022</v>
       </c>
       <c r="D150" t="n">
-        <v>0</v>
+        <v>1067.31920298573</v>
       </c>
       <c r="E150" t="n">
-        <v>0</v>
+        <v>32.4764193443842</v>
       </c>
       <c r="F150" t="n">
         <v>342.317561623989</v>
@@ -31978,10 +32036,10 @@
         <v>339.683180551829</v>
       </c>
       <c r="H150" t="n">
-        <v>342.317561623989</v>
+        <v>1409.63676460972</v>
       </c>
       <c r="I150" t="n">
-        <v>339.683180551829</v>
+        <v>341.232151127702</v>
       </c>
     </row>
     <row r="151">
@@ -31995,10 +32053,10 @@
         <v>2023</v>
       </c>
       <c r="D151" t="n">
-        <v>9.35164835164836</v>
+        <v>803.79525817775</v>
       </c>
       <c r="E151" t="n">
-        <v>1.65114810539119</v>
+        <v>24.4579051876734</v>
       </c>
       <c r="F151" t="n">
         <v>265.288387978145</v>
@@ -32007,10 +32065,10 @@
         <v>263.40537918255</v>
       </c>
       <c r="H151" t="n">
-        <v>274.640036329794</v>
+        <v>1069.0836461559</v>
       </c>
       <c r="I151" t="n">
-        <v>263.410554215978</v>
+        <v>264.538433707603</v>
       </c>
     </row>
   </sheetData>

</xml_diff>